<commit_message>
fix: add missing stats file and generate tables and graphs again
</commit_message>
<xml_diff>
--- a/tables/O3CPU/RISCV/O3CPU_RISCV_PARSEC_PdR_Dcache-hits.xlsx
+++ b/tables/O3CPU/RISCV/O3CPU_RISCV_PARSEC_PdR_Dcache-hits.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -660,6 +660,21 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>LFU</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>31101562</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>TournamentBP</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>